<commit_message>
parking fee final test doc
</commit_message>
<xml_diff>
--- a/parking fee software.xlsx
+++ b/parking fee software.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testing work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96A4FB-55AC-42F8-B54A-56D9C945E10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5F1A2A-EAB7-4FE2-9B80-EC686A4ACC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="2" r:id="rId1"/>
     <sheet name="valet parking" sheetId="1" r:id="rId2"/>
     <sheet name="short term parking" sheetId="3" r:id="rId3"/>
     <sheet name="Economy parking" sheetId="4" r:id="rId4"/>
+    <sheet name="Long term garage parking" sheetId="5" r:id="rId5"/>
+    <sheet name="Long term surface parking" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="156">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -442,6 +444,196 @@
   </si>
   <si>
     <t>TC_EP_005</t>
+  </si>
+  <si>
+    <t>TC_EP_006</t>
+  </si>
+  <si>
+    <t>estimated parking cost =2</t>
+  </si>
+  <si>
+    <t>TC_EP_007</t>
+  </si>
+  <si>
+    <t>validate logic of daily parking</t>
+  </si>
+  <si>
+    <t>estimated cost should be 9</t>
+  </si>
+  <si>
+    <t>TC_EP_008</t>
+  </si>
+  <si>
+    <t>validate weekly parking logic</t>
+  </si>
+  <si>
+    <t>1.go to website
+2.click on input field of "entry date and time"
+3.enter data1
+4.click on input field of entry time.
+5. input data2
+6.select PM on radio button
+7.click on input field of "leaving date and time"
+8.enter data3
+9.click on input field of entry time.
+10. input data4
+11.select PM on radio button
+12.click calculate</t>
+  </si>
+  <si>
+    <t>1.goto website
+2.click on input field of "entry date and time"
+3.enter data1
+4.click on input field of entry time.
+5. input data2
+6.select PM on radio button
+7.click on input field of "leaving date and time"
+8.enter data3
+9.click on input field of entry time.
+10. input data4
+11.select PM on radio button
+12.click calculate</t>
+  </si>
+  <si>
+    <t>estimated cost should be 54</t>
+  </si>
+  <si>
+    <t>data1: 13/5/2025
+data2: 12:00
+data3: 20/5/2025
+data4: 12:00</t>
+  </si>
+  <si>
+    <t>estimated parking cost =9</t>
+  </si>
+  <si>
+    <t>estimated parking cost =54</t>
+  </si>
+  <si>
+    <t>TC_LGP_001</t>
+  </si>
+  <si>
+    <t>TS_004
+(Long term garage parking)</t>
+  </si>
+  <si>
+    <t>1.Go to the website
+2.check the choose parking lot dropdown box and  select as long term garage paraking
+3.check click calculate without any datas</t>
+  </si>
+  <si>
+    <t>1.in the choose parking dropdown list long term garage parking  should be already selected
+2.estimated parking costs should be 0.</t>
+  </si>
+  <si>
+    <t>TC_LGP_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.in the dropdown list long term garage parking parking is  selected
+2.page is not loading when we click calculate without any data
+</t>
+  </si>
+  <si>
+    <t>TC_LGP_003</t>
+  </si>
+  <si>
+    <t>TC_LGP_004</t>
+  </si>
+  <si>
+    <t>TC_LGP_005</t>
+  </si>
+  <si>
+    <t>TC_LGP_006</t>
+  </si>
+  <si>
+    <t>TC_LGP_007</t>
+  </si>
+  <si>
+    <t>validate daily maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Go to website
+2.click on input field of "entry date and time"
+3.enter data1
+4.click on input field of entry time.
+5. input data2
+6.select PM on radio button
+7.click on input field of "leaving date and time"
+8.enter data3
+9.click on input field of entry time.
+10. input data4
+11.select PM on radio button
+12.click calculate
+</t>
+  </si>
+  <si>
+    <t>1.when we click calculate
+"Estimated parking costs" should be "10"</t>
+  </si>
+  <si>
+    <t>estimated parking cost =12</t>
+  </si>
+  <si>
+    <t>TC_LGP_008</t>
+  </si>
+  <si>
+    <t>validate weekly maximum</t>
+  </si>
+  <si>
+    <t>1.when we click calculate
+"Estimated parking costs" should be "72"</t>
+  </si>
+  <si>
+    <t>estimated parking cost =72</t>
+  </si>
+  <si>
+    <t>TC_LGSP_001</t>
+  </si>
+  <si>
+    <t>1.Go to the website
+2.check the choose parking lot dropdown box and  select as long term surface parking
+3.check click calculate without any datas</t>
+  </si>
+  <si>
+    <t>1.in the choose parking dropdown list long term surface parking  should be already selected
+2.estimated parking costs should be 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.in the dropdown list long term surface  parking is  selected
+2.page is not loading when we click calculate without any data
+</t>
+  </si>
+  <si>
+    <t>TC_LGSP_002</t>
+  </si>
+  <si>
+    <t>TS_005
+(Long term surface parking)</t>
+  </si>
+  <si>
+    <t>TC_LGSP_003</t>
+  </si>
+  <si>
+    <t>TC_LGSP_004</t>
+  </si>
+  <si>
+    <t>TC_LGSP_005</t>
+  </si>
+  <si>
+    <t>TC_LGSP_006</t>
+  </si>
+  <si>
+    <t>TC_LGSP_007</t>
+  </si>
+  <si>
+    <t>estimated parking cost =10</t>
+  </si>
+  <si>
+    <t>1.when we click calculate
+"Estimated parking costs" should be "60"</t>
+  </si>
+  <si>
+    <t>estimated parking cost =60</t>
   </si>
 </sst>
 </file>
@@ -1443,8 +1635,8 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:H6"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,9 +1956,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EAF263-A97A-4FCF-9E8D-19A2CCEAAA71}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1963,45 +2155,89 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="223.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="C7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+    <row r="8" spans="1:11" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+    <row r="9" spans="1:11" ht="226.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -2286,6 +2522,612 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{A731703E-F3CD-46B3-BF99-10A3AFDBA1E6}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{392D4996-33AE-4610-ACBE-7070403477C1}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{8A32D4D7-78BE-485E-AA0C-6E26D57C76AB}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{47DB70B4-5950-4595-B3A0-4FD158DA6510}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{C9B96A04-3022-4554-AB48-7FF78C448BBD}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{BD18DEEF-D48F-4773-8D52-193499E6BE63}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A68B14-C2AE-447F-98DF-9B71F7C87AD4}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="9" customFormat="1" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="9" customFormat="1" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="9" customFormat="1" ht="164.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="9" customFormat="1" ht="223.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="9" customFormat="1" ht="245.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="9" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D6F3F896-EFFB-43A4-A06C-31C995B431E7}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{EA90B6BE-D366-4182-8844-8F3CDFE5B560}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{87B4F61B-38C2-4217-9077-32D826FB7867}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{4048940B-0EC9-4884-8675-7F4D4FFAD016}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{0E7201BF-06E2-4A2D-AF8B-F8FCA05CBE23}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{2CBFD59A-9BD4-4135-9800-03EDD03F4D85}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{D0E05BFD-2C43-4AA3-9003-6BAE08F24367}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{A86B53A6-6F8F-4D7E-8F9B-D77BDC5B618A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F2DCBD-1732-4020-8F6B-05E75141A5D6}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="9" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="9" customFormat="1" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="9" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="9" customFormat="1" ht="142.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="164.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="9" customFormat="1" ht="217.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="9" customFormat="1" ht="212.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="187.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{DE738274-D1C4-4F68-9ED7-EEE70FD59E45}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{90CD1AFF-BBE4-49FA-BAD3-FAA6399D62B6}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{EEC9B9DF-937C-421C-87B4-574BE3E3ECB0}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{9C2CEA8D-56F0-4914-991E-1B2809120704}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{4936134C-431C-4110-AF9F-5DE53DEF09B7}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{46F2BD3C-D4E7-48D7-B0BE-6662BA3CE8B4}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{50A6A74F-8611-4489-9698-042CAA235AD5}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{8B310DB9-E2CB-46E2-A582-159599E006AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>